<commit_message>
consertando erros de escrita
</commit_message>
<xml_diff>
--- a/data/raw data/Lista de Palestras.xlsx
+++ b/data/raw data/Lista de Palestras.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\Documentos\Pos-Graduacao\Pós-Doutorado\palestrasppgeufrj\data\raw data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="20500" windowHeight="7900"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
   <si>
     <t>Dia</t>
   </si>
@@ -71,9 +69,6 @@
     <t>Extrangeira</t>
   </si>
   <si>
-    <t>University of Connectivut</t>
-  </si>
-  <si>
     <t>Professor</t>
   </si>
   <si>
@@ -258,15 +253,57 @@
   </si>
   <si>
     <t>Horario</t>
+  </si>
+  <si>
+    <r>
+      <t>University of Connecti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ut</t>
+    </r>
+  </si>
+  <si>
+    <t>Misturado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -308,16 +345,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -379,7 +422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,7 +457,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,7 +634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -601,36 +644,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="134" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -663,16 +708,16 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -698,31 +743,31 @@
         <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O2" s="1">
         <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -736,43 +781,43 @@
         <v>2016</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="O3" s="1">
         <v>16</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -786,43 +831,43 @@
         <v>2016</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="1">
         <v>16</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -836,43 +881,43 @@
         <v>2016</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="1">
         <v>16</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -886,43 +931,43 @@
         <v>2016</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="O6" s="1">
         <v>16</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -936,43 +981,43 @@
         <v>2016</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O7" s="1">
         <v>16</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -986,43 +1031,43 @@
         <v>2016</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O8" s="1">
         <v>16</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1036,43 +1081,43 @@
         <v>2016</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O9" s="1">
         <v>16</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1086,43 +1131,43 @@
         <v>2016</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O10" s="1">
         <v>16</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1136,43 +1181,43 @@
         <v>2016</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O11" s="1">
         <v>16</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1186,43 +1231,43 @@
         <v>2016</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="N12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O12" s="1">
         <v>16</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1236,44 +1281,49 @@
         <v>2016</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>63</v>
+      <c r="L13" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O13" s="1">
         <v>16</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionando mais informações sobre as ultimas palestras
</commit_message>
<xml_diff>
--- a/data/raw data/Lista de Palestras.xlsx
+++ b/data/raw data/Lista de Palestras.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\Documentos\Pos-Graduacao\Pós-Doutorado\palestrasppgeufrj\data\raw data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="5240" yWindow="1600" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="150">
   <si>
     <t>Dia</t>
   </si>
@@ -393,30 +388,99 @@
   </si>
   <si>
     <t>O deficit Eltoniano e a visao Grinneliana - a ecologia funcional entre os desajustes conceituais de nicho</t>
+  </si>
+  <si>
+    <t>Miguel Angel Rodríguez-Gironés Arboli</t>
+  </si>
+  <si>
+    <t>Crab spider colouration: function and evolution</t>
+  </si>
+  <si>
+    <t>Thaise Emílio Lopes de Sousa</t>
+  </si>
+  <si>
+    <t>Hiperdominância e declinio de palmeiras nas florestas da Amazonia</t>
+  </si>
+  <si>
+    <t>Royal Botanic Gardens</t>
+  </si>
+  <si>
+    <t>Populacoes de Plantas</t>
+  </si>
+  <si>
+    <t>Sandra Azevedo</t>
+  </si>
+  <si>
+    <t>Cianobactérias tóxicas: um exemplo de inter-relação entre ambiente e saúde</t>
+  </si>
+  <si>
+    <t>Impactos Antropicos</t>
+  </si>
+  <si>
+    <t>Leandro Dumas</t>
+  </si>
+  <si>
+    <t>Deu Zebra! A fauna brasileira representada nos símbolos dos clubes de futebol do país</t>
+  </si>
+  <si>
+    <t>Entomologia</t>
+  </si>
+  <si>
+    <t>Zoologia Cultural</t>
+  </si>
+  <si>
+    <t>Daniele Kasper</t>
+  </si>
+  <si>
+    <t>O ciclo do mercúrio em ecossistemas aquáticos amazônicos</t>
+  </si>
+  <si>
+    <t>Radioisotopos</t>
+  </si>
+  <si>
+    <t>Biogeoquimica</t>
+  </si>
+  <si>
+    <t>Panorama da Área e o Mestrado Profissional em Biodiversidade</t>
+  </si>
+  <si>
+    <t>Leandro Freitas</t>
+  </si>
+  <si>
+    <t>JBRJ</t>
+  </si>
+  <si>
+    <t>Polinizacao</t>
+  </si>
+  <si>
+    <t>Pos-Graduacao</t>
+  </si>
+  <si>
+    <t>André Braga Junqueira</t>
+  </si>
+  <si>
+    <t>Ecologia histórica da Amazônia: heranças pré-Colombianas nas florestas e nos sistemas agrícolas atuais</t>
+  </si>
+  <si>
+    <t>Ecologia Historica</t>
+  </si>
+  <si>
+    <t>Marcus Vinicius Vieira</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Estación Experimental de Zonas Áridas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -438,6 +502,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -456,101 +534,132 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="38" builtinId="9" hidden="1"/>
+  <cellStyles count="53">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -821,7 +930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -829,34 +938,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="134" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -909,7 +1018,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -962,7 +1071,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1015,7 +1124,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1068,7 +1177,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1121,7 +1230,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1174,7 +1283,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1227,7 +1336,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1280,7 +1389,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1333,7 +1442,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1386,7 +1495,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1439,7 +1548,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1492,7 +1601,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1545,7 +1654,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1598,7 +1707,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1651,7 +1760,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1704,7 +1813,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1757,7 +1866,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1810,7 +1919,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1863,7 +1972,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1916,7 +2025,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1969,9 +2078,433 @@
         <v>111</v>
       </c>
     </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O22" s="2">
+        <v>12</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>23</v>
+      </c>
+      <c r="C23" s="2">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O23" s="2">
+        <v>12</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O24" s="2">
+        <v>12</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2">
+        <v>9</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O25" s="2">
+        <v>12</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>20</v>
+      </c>
+      <c r="C26" s="2">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O26" s="2">
+        <v>12</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O27" s="2">
+        <v>12</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O28" s="2">
+        <v>12</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>